<commit_message>
upate case-log.xlsx add one week
</commit_message>
<xml_diff>
--- a/cases-log.xlsx
+++ b/cases-log.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" hidePivotFieldList="1"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
   </bookViews>
@@ -20,11 +20,11 @@
     <definedName name="rate_cg">'work log-monthly'!$X$12</definedName>
     <definedName name="rate_table">'work log-monthly'!$W$6:$X$12</definedName>
     <definedName name="today">'work log-monthly'!$J$2</definedName>
-    <definedName name="WeekStart" localSheetId="0">'work log-monthly'!$L$2</definedName>
+    <definedName name="WeekStart" localSheetId="0">'work log-monthly'!$K$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId2"/>
+    <pivotCache cacheId="18" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>MON</t>
   </si>
@@ -95,10 +95,6 @@
   </si>
   <si>
     <t>Monthly Start</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>Today</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
@@ -188,6 +184,10 @@
   </si>
   <si>
     <t>14:20~15:20</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Today</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -336,7 +336,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +406,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,6 +614,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -629,14 +638,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -685,12 +688,6 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -701,6 +698,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -735,27 +741,27 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="作者" refreshedDate="45076.531363657406" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="18">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="作者" refreshedDate="45076.601096759259" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="24">
   <cacheSource type="worksheet">
-    <worksheetSource ref="Q6:S24" sheet="work log-monthly"/>
+    <worksheetSource ref="Q5:S29" sheet="work log-monthly"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Case" numFmtId="0">
       <sharedItems containsBlank="1" count="7">
+        <m/>
         <s v="ca"/>
         <s v="cb"/>
         <s v="cc"/>
-        <m/>
         <s v="cd"/>
         <s v="cf"/>
         <s v="ce"/>
       </sharedItems>
     </cacheField>
     <cacheField name="wh_subt" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="4"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
     </cacheField>
     <cacheField name="sub1_rev" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="12000"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1000" maxValue="12500"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -767,39 +773,44 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="18">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="24">
   <r>
     <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
     <n v="3"/>
     <n v="6000"/>
   </r>
   <r>
-    <x v="1"/>
-    <n v="4"/>
-    <n v="10000"/>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="12500"/>
   </r>
   <r>
-    <x v="2"/>
+    <x v="3"/>
     <n v="4"/>
     <n v="12000"/>
   </r>
   <r>
-    <x v="3"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
+    <x v="0"/>
     <m/>
     <m/>
   </r>
   <r>
     <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
     <n v="2"/>
     <n v="4000"/>
   </r>
   <r>
-    <x v="1"/>
+    <x v="2"/>
     <n v="1"/>
     <n v="2500"/>
   </r>
@@ -809,24 +820,24 @@
     <n v="7000"/>
   </r>
   <r>
-    <x v="3"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
+    <x v="0"/>
     <m/>
     <m/>
   </r>
   <r>
     <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
     <n v="2"/>
     <n v="4000"/>
   </r>
   <r>
-    <x v="2"/>
-    <n v="0"/>
-    <n v="0"/>
+    <x v="4"/>
+    <n v="2"/>
+    <n v="7000"/>
   </r>
   <r>
     <x v="5"/>
@@ -834,22 +845,47 @@
     <n v="1000"/>
   </r>
   <r>
-    <x v="3"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
+    <x v="0"/>
     <m/>
     <m/>
   </r>
   <r>
     <x v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <m/>
+    <m/>
   </r>
   <r>
     <x v="1"/>
+    <n v="1"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="5000"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3"/>
+    <n v="4500"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="2"/>
     <n v="2"/>
     <n v="5000"/>
   </r>
@@ -862,18 +898,18 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="樞紐分析表1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="數值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="樞紐分析表2" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="數值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="W16:Y24" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
       <items count="8">
-        <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item x="3"/>
         <item x="4"/>
         <item x="6"/>
         <item x="5"/>
-        <item x="3"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -921,8 +957,8 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="加總 - wh_subt" fld="1" baseField="0" baseItem="3"/>
-    <dataField name="加總 - sub1_rev" fld="2" baseField="0" baseItem="3"/>
+    <dataField name="加總 - wh_subt" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="加總 - sub1_rev" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1141,8 +1177,8 @@
   </sheetPr>
   <dimension ref="B1:AI59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1157,8 +1193,8 @@
     <col min="20" max="20" width="7.5" style="3" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="6.125" style="3" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="2.875" style="3" customWidth="1"/>
-    <col min="23" max="23" width="9.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="15.5" style="3" customWidth="1"/>
     <col min="25" max="25" width="16.375" style="3" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.625" style="3" customWidth="1"/>
     <col min="27" max="27" width="8.5" style="3" customWidth="1"/>
@@ -1177,49 +1213,50 @@
       <c r="B1" s="2"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="22"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="2:25" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="37">
+      <c r="B2" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="36">
         <f ca="1">MONTH(monthlystart)</f>
         <v>5</v>
       </c>
-      <c r="F2" s="37"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="24"/>
       <c r="H2" s="24">
         <f ca="1">EOMONTH(today,-1)+1</f>
         <v>45047</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25">
-        <f ca="1">TODAY()</f>
+      <c r="I2" s="16"/>
+      <c r="J2" s="24">
+        <f t="shared" ref="J2" ca="1" si="0">TODAY()</f>
         <v>45076</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25">
-        <f ca="1">monthlystart-WEEKDAY(TODAY(),2)+1</f>
-        <v>45046</v>
-      </c>
+      <c r="K2" s="46">
+        <f ca="1">monthlystart-WEEKDAY(TODAY(),2)+2</f>
+        <v>45047</v>
+      </c>
+      <c r="L2" s="46"/>
+      <c r="P2" s="16"/>
     </row>
     <row r="3" spans="2:25" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7"/>
@@ -1246,34 +1283,34 @@
     </row>
     <row r="4" spans="2:25" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="13"/>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16" t="s">
+      <c r="H4" s="17"/>
+      <c r="I4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16" t="s">
+      <c r="J4" s="17"/>
+      <c r="K4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="17" t="s">
+      <c r="L4" s="17"/>
+      <c r="M4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17" t="s">
+      <c r="N4" s="18"/>
+      <c r="O4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="17"/>
+      <c r="P4" s="18"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
@@ -1285,49 +1322,49 @@
     </row>
     <row r="5" spans="2:25" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
-      <c r="C5" s="18" t="str">
+      <c r="C5" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+0,"mmm dd"))</f>
-        <v>Apr 30</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18" t="str">
+        <v>May 01</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+1,"mmm dd"))</f>
-        <v>May 01</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="str">
+        <v>May 02</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+2,"mmm dd"))</f>
-        <v>May 02</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18" t="str">
+        <v>May 03</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+3,"mmm dd"))</f>
-        <v>May 03</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18" t="str">
+        <v>May 04</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+4,"mmm dd"))</f>
-        <v>May 04</v>
-      </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="20" t="str">
+        <v>May 05</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="M5" s="21" t="str">
         <f ca="1">(TEXT(WeekStart+5,"mmm dd"))</f>
-        <v>May 05</v>
-      </c>
-      <c r="N5" s="19"/>
-      <c r="O5" s="21" t="str">
+        <v>May 06</v>
+      </c>
+      <c r="N5" s="20"/>
+      <c r="O5" s="22" t="str">
         <f ca="1">(TEXT(WeekStart+6,"mmm dd"))</f>
-        <v>May 06</v>
-      </c>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="43" t="s">
+        <v>May 07</v>
+      </c>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="44" t="s">
+      <c r="S5" s="48" t="s">
         <v>27</v>
-      </c>
-      <c r="S5" s="44" t="s">
-        <v>28</v>
       </c>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
@@ -1336,76 +1373,76 @@
       <c r="X5" s="14"/>
     </row>
     <row r="6" spans="2:25" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="33">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="32">
         <f>SUM(D7:D9)</f>
         <v>1</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="33">
+      <c r="E6" s="25"/>
+      <c r="F6" s="32">
         <f>SUM(F7:F9)</f>
         <v>2</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="33">
+      <c r="G6" s="25"/>
+      <c r="H6" s="32">
         <f>SUM(H7:H9)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="33">
+      <c r="I6" s="25"/>
+      <c r="J6" s="32">
         <f>SUM(J7:J9)</f>
         <v>3</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="33">
+      <c r="K6" s="25"/>
+      <c r="L6" s="32">
         <f>SUM(L7:L9)</f>
         <v>2</v>
       </c>
-      <c r="M6" s="26"/>
-      <c r="N6" s="33">
+      <c r="M6" s="25"/>
+      <c r="N6" s="32">
         <f>SUM(N7:N9)</f>
         <v>2</v>
       </c>
-      <c r="O6" s="26"/>
-      <c r="P6" s="33">
+      <c r="O6" s="25"/>
+      <c r="P6" s="32">
         <f>SUM(P7:P9)</f>
         <v>2</v>
       </c>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
       <c r="T6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="U6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34" t="s">
-        <v>18</v>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="27">
+      <c r="C7" s="42"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="26">
         <v>2</v>
       </c>
-      <c r="M7" s="46"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="30">
+      <c r="M7" s="43"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="29">
         <v>1</v>
       </c>
       <c r="Q7" s="3" t="str">
@@ -1416,8 +1453,8 @@
         <f>SUM(D7,F7,H7,J7,L7,N7,P7)</f>
         <v>3</v>
       </c>
-      <c r="S7" s="42">
-        <f>T7*R7</f>
+      <c r="S7" s="41">
+        <f t="shared" ref="S7:S9" si="1">LOOKUP(Q7,$W$7:$X$12)*R7</f>
         <v>6000</v>
       </c>
       <c r="T7" s="3">
@@ -1428,10 +1465,10 @@
         <f>INDEX($X$7:$X$12,MATCH(Q7,$W$7:$W$12,0))</f>
         <v>2000</v>
       </c>
-      <c r="W7" s="35" t="s">
+      <c r="W7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="X7" s="36">
+      <c r="X7" s="35">
         <v>2000</v>
       </c>
     </row>
@@ -1439,40 +1476,40 @@
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="28">
+      <c r="C8" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="27">
         <v>1</v>
       </c>
-      <c r="E8" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="28">
+      <c r="E8" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="27">
         <v>2</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="31">
+      <c r="G8" s="42"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="30">
         <v>2</v>
       </c>
-      <c r="O8" s="47"/>
-      <c r="P8" s="31"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="30"/>
       <c r="Q8" s="3" t="str">
-        <f t="shared" ref="Q8:Q9" si="0">B8</f>
+        <f t="shared" ref="Q8:Q9" si="2">B8</f>
         <v>cb</v>
       </c>
       <c r="R8" s="3">
         <f>SUM(D8,F8,H8,J8,L8,N8,P8)</f>
         <v>5</v>
       </c>
-      <c r="S8" s="42">
-        <f t="shared" ref="S8:S9" si="1">LOOKUP(Q8,$W$7:$X$12)*R8</f>
+      <c r="S8" s="41">
+        <f t="shared" si="1"/>
         <v>12500</v>
       </c>
       <c r="T8" s="3">
@@ -1480,13 +1517,13 @@
         <v>2500</v>
       </c>
       <c r="U8" s="3">
-        <f t="shared" ref="U8:U9" si="2">INDEX($X$7:$X$12,MATCH(Q8,$W$7:$W$12,0))</f>
+        <f t="shared" ref="U8:U9" si="3">INDEX($X$7:$X$12,MATCH(Q8,$W$7:$W$12,0))</f>
         <v>2500</v>
       </c>
-      <c r="W8" s="35" t="s">
+      <c r="W8" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="X8" s="36">
+      <c r="X8" s="35">
         <v>2500</v>
       </c>
     </row>
@@ -1494,33 +1531,33 @@
       <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="29">
+      <c r="C9" s="42"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="28">
         <v>3</v>
       </c>
-      <c r="K9" s="45"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="32">
+      <c r="K9" s="42"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="45"/>
+      <c r="P9" s="31">
         <v>1</v>
       </c>
       <c r="Q9" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>cc</v>
       </c>
       <c r="R9" s="3">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9)</f>
         <v>4</v>
       </c>
-      <c r="S9" s="42">
+      <c r="S9" s="41">
         <f t="shared" si="1"/>
         <v>12000</v>
       </c>
@@ -1529,82 +1566,82 @@
         <v>3000</v>
       </c>
       <c r="U9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3000</v>
       </c>
-      <c r="W9" s="35" t="s">
+      <c r="W9" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="X9" s="36">
+      <c r="X9" s="35">
         <v>3000</v>
       </c>
     </row>
     <row r="10" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
-      <c r="C10" s="18" t="str">
+      <c r="C10" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+0+7,"mmm dd"))</f>
-        <v>May 07</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18" t="str">
+        <v>May 08</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+1+7,"mmm dd"))</f>
-        <v>May 08</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18" t="str">
+        <v>May 09</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+2+7,"mmm dd"))</f>
-        <v>May 09</v>
-      </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18" t="str">
+        <v>May 10</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+3+7,"mmm dd"))</f>
-        <v>May 10</v>
-      </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18" t="str">
+        <v>May 11</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+4+7,"mmm dd"))</f>
-        <v>May 11</v>
-      </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="20" t="str">
+        <v>May 12</v>
+      </c>
+      <c r="L10" s="19"/>
+      <c r="M10" s="21" t="str">
         <f ca="1">(TEXT(WeekStart+5+7,"mmm dd"))</f>
-        <v>May 12</v>
-      </c>
-      <c r="N10" s="19"/>
-      <c r="O10" s="21" t="str">
+        <v>May 13</v>
+      </c>
+      <c r="N10" s="20"/>
+      <c r="O10" s="22" t="str">
         <f ca="1">(TEXT(WeekStart+6+7,"mmm dd"))</f>
-        <v>May 13</v>
-      </c>
-      <c r="P10" s="19"/>
-      <c r="S10" s="42"/>
-      <c r="W10" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="X10" s="36">
+        <v>May 14</v>
+      </c>
+      <c r="P10" s="20"/>
+      <c r="S10" s="41"/>
+      <c r="W10" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="X10" s="35">
         <v>3500</v>
       </c>
     </row>
     <row r="11" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="S11" s="42"/>
-      <c r="W11" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="X11" s="36">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="S11" s="41"/>
+      <c r="W11" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="X11" s="35">
         <v>1500</v>
       </c>
     </row>
@@ -1612,22 +1649,22 @@
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="27">
+      <c r="C12" s="42"/>
+      <c r="D12" s="26">
         <v>2</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="30"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="29"/>
       <c r="Q12" s="3" t="str">
         <f>B12</f>
         <v>ca</v>
@@ -1636,7 +1673,7 @@
         <f>SUM(D12,F12,H12,J12,L12,N12,P12)</f>
         <v>2</v>
       </c>
-      <c r="S12" s="42">
+      <c r="S12" s="41">
         <f>LOOKUP(Q12,$W$7:$X$12)*R12</f>
         <v>4000</v>
       </c>
@@ -1648,10 +1685,10 @@
         <f>INDEX($X$7:$X$12,MATCH(Q12,$W$7:$W$12,0))</f>
         <v>2000</v>
       </c>
-      <c r="W12" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="X12" s="36">
+      <c r="W12" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="X12" s="35">
         <v>1000</v>
       </c>
     </row>
@@ -1659,32 +1696,32 @@
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="28">
+      <c r="C13" s="42"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="27">
         <v>1</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="31"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="30"/>
       <c r="Q13" s="3" t="str">
-        <f t="shared" ref="Q13:Q14" si="3">B13</f>
+        <f t="shared" ref="Q13:Q14" si="4">B13</f>
         <v>cb</v>
       </c>
       <c r="R13" s="3">
         <f>SUM(D13,F13,H13,J13,L13,N13,P13)</f>
         <v>1</v>
       </c>
-      <c r="S13" s="42">
-        <f t="shared" ref="S13:S14" si="4">LOOKUP(Q13,$W$7:$X$12)*R13</f>
+      <c r="S13" s="41">
+        <f t="shared" ref="S13:S14" si="5">LOOKUP(Q13,$W$7:$X$12)*R13</f>
         <v>2500</v>
       </c>
       <c r="T13" s="3">
@@ -1692,40 +1729,40 @@
         <v>2500</v>
       </c>
       <c r="U13" s="3">
-        <f t="shared" ref="U13:U14" si="5">INDEX($X$7:$X$12,MATCH(Q13,$W$7:$W$12,0))</f>
+        <f t="shared" ref="U13:U14" si="6">INDEX($X$7:$X$12,MATCH(Q13,$W$7:$W$12,0))</f>
         <v>2500</v>
       </c>
     </row>
     <row r="14" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="29">
+        <v>21</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="28">
         <v>2</v>
       </c>
-      <c r="I14" s="45"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="32"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="31"/>
       <c r="Q14" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cd</v>
       </c>
       <c r="R14" s="3">
         <f>SUM(D14,F14,H14,J14,L14,N14,P14)</f>
         <v>2</v>
       </c>
-      <c r="S14" s="42">
-        <f t="shared" si="4"/>
+      <c r="S14" s="41">
+        <f t="shared" si="5"/>
         <v>7000</v>
       </c>
       <c r="T14" s="3">
@@ -1733,96 +1770,96 @@
         <v>3500</v>
       </c>
       <c r="U14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3500</v>
       </c>
     </row>
     <row r="15" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15"/>
-      <c r="C15" s="18" t="str">
+      <c r="C15" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+0+14,"mmm dd"))</f>
-        <v>May 14</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18" t="str">
+        <v>May 15</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+1+14,"mmm dd"))</f>
-        <v>May 15</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18" t="str">
+        <v>May 16</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+2+14,"mmm dd"))</f>
-        <v>May 16</v>
-      </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18" t="str">
+        <v>May 17</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+3+14,"mmm dd"))</f>
-        <v>May 17</v>
-      </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18" t="str">
+        <v>May 18</v>
+      </c>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+4+14,"mmm dd"))</f>
-        <v>May 18</v>
-      </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="20" t="str">
+        <v>May 19</v>
+      </c>
+      <c r="L15" s="19"/>
+      <c r="M15" s="21" t="str">
         <f ca="1">(TEXT(WeekStart+5+14,"mmm dd"))</f>
-        <v>May 19</v>
-      </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="21" t="str">
+        <v>May 20</v>
+      </c>
+      <c r="N15" s="20"/>
+      <c r="O15" s="22" t="str">
         <f ca="1">(TEXT(WeekStart+6+14,"mmm dd"))</f>
-        <v>May 20</v>
-      </c>
-      <c r="P15" s="19"/>
-      <c r="S15" s="42"/>
+        <v>May 21</v>
+      </c>
+      <c r="P15" s="20"/>
+      <c r="S15" s="41"/>
     </row>
     <row r="16" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="S16" s="42"/>
-      <c r="W16" s="39" t="s">
-        <v>33</v>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="S16" s="41"/>
+      <c r="W16" s="38" t="s">
+        <v>32</v>
       </c>
       <c r="X16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="27">
+      <c r="C17" s="42"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="26">
         <v>2</v>
       </c>
-      <c r="I17" s="45"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="30"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="29"/>
       <c r="Q17" s="3" t="str">
         <f>B17</f>
         <v>ca</v>
@@ -1831,7 +1868,7 @@
         <f>SUM(D17,F17,H17,J17,L17,N17,P17)</f>
         <v>2</v>
       </c>
-      <c r="S17" s="42">
+      <c r="S17" s="41">
         <f>LOOKUP(Q17,$W$7:$X$12)*R17</f>
         <v>4000</v>
       </c>
@@ -1843,94 +1880,96 @@
         <f>INDEX($X$7:$X$12,MATCH(Q17,$W$7:$W$12,0))</f>
         <v>2000</v>
       </c>
-      <c r="W17" s="40" t="s">
+      <c r="W17" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="X17" s="41">
-        <v>7</v>
-      </c>
-      <c r="Y17" s="41">
-        <v>14000</v>
+      <c r="X17" s="40">
+        <v>9</v>
+      </c>
+      <c r="Y17" s="40">
+        <v>18000</v>
       </c>
     </row>
     <row r="18" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="31"/>
+        <v>21</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="27">
+        <v>2</v>
+      </c>
+      <c r="E18" s="42"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="30"/>
       <c r="Q18" s="3" t="str">
-        <f t="shared" ref="Q18:Q19" si="6">B18</f>
+        <f t="shared" ref="Q18:Q19" si="7">B18</f>
         <v>cd</v>
       </c>
       <c r="R18" s="3">
         <f>SUM(D18,F18,H18,J18,L18,N18,P18)</f>
-        <v>0</v>
-      </c>
-      <c r="S18" s="42">
-        <f t="shared" ref="S18:S19" si="7">LOOKUP(Q18,$W$7:$X$12)*R18</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="S18" s="41">
+        <f t="shared" ref="S18:S19" si="8">LOOKUP(Q18,$W$7:$X$12)*R18</f>
+        <v>7000</v>
       </c>
       <c r="T18" s="3">
         <f>LOOKUP(Q18,$W$7:$X$12)</f>
         <v>3500</v>
       </c>
       <c r="U18" s="3">
-        <f t="shared" ref="U18:U19" si="8">INDEX($X$7:$X$12,MATCH(Q18,$W$7:$W$12,0))</f>
+        <f t="shared" ref="U18:U19" si="9">INDEX($X$7:$X$12,MATCH(Q18,$W$7:$W$12,0))</f>
         <v>3500</v>
       </c>
-      <c r="W18" s="40" t="s">
+      <c r="W18" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="X18" s="41">
-        <v>7</v>
-      </c>
-      <c r="Y18" s="41">
-        <v>17500</v>
+      <c r="X18" s="40">
+        <v>10</v>
+      </c>
+      <c r="Y18" s="40">
+        <v>25000</v>
       </c>
     </row>
     <row r="19" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="29">
+        <v>22</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="28">
         <v>1</v>
       </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="32"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="31"/>
       <c r="Q19" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>cf</v>
       </c>
       <c r="R19" s="3">
         <f>SUM(D19,F19,H19,J19,L19,N19,P19)</f>
         <v>1</v>
       </c>
-      <c r="S19" s="42">
-        <f t="shared" si="7"/>
+      <c r="S19" s="41">
+        <f t="shared" si="8"/>
         <v>1000</v>
       </c>
       <c r="T19" s="3">
@@ -1938,123 +1977,125 @@
         <v>1000</v>
       </c>
       <c r="U19" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1000</v>
       </c>
-      <c r="W19" s="40" t="s">
+      <c r="W19" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="X19" s="41">
+      <c r="X19" s="40">
         <v>4</v>
       </c>
-      <c r="Y19" s="41">
+      <c r="Y19" s="40">
         <v>12000</v>
       </c>
     </row>
     <row r="20" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
-      <c r="C20" s="18" t="str">
+      <c r="C20" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+0+21,"mmm dd"))</f>
-        <v>May 21</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18" t="str">
+        <v>May 22</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+1+21,"mmm dd"))</f>
-        <v>May 22</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18" t="str">
+        <v>May 23</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+2+21,"mmm dd"))</f>
-        <v>May 23</v>
-      </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18" t="str">
+        <v>May 24</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+3+21,"mmm dd"))</f>
-        <v>May 24</v>
-      </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18" t="str">
+        <v>May 25</v>
+      </c>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19" t="str">
         <f ca="1">(TEXT(WeekStart+4+21,"mmm dd"))</f>
-        <v>May 25</v>
-      </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="20" t="str">
+        <v>May 26</v>
+      </c>
+      <c r="L20" s="19"/>
+      <c r="M20" s="21" t="str">
         <f ca="1">(TEXT(WeekStart+5+21,"mmm dd"))</f>
-        <v>May 26</v>
-      </c>
-      <c r="N20" s="19"/>
-      <c r="O20" s="21" t="str">
+        <v>May 27</v>
+      </c>
+      <c r="N20" s="20"/>
+      <c r="O20" s="22" t="str">
         <f ca="1">(TEXT(WeekStart+6+21,"mmm dd"))</f>
-        <v>May 27</v>
-      </c>
-      <c r="P20" s="19"/>
-      <c r="S20" s="42"/>
-      <c r="W20" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="X20" s="41">
-        <v>2</v>
-      </c>
-      <c r="Y20" s="41">
-        <v>7000</v>
+        <v>May 28</v>
+      </c>
+      <c r="P20" s="20"/>
+      <c r="S20" s="41"/>
+      <c r="W20" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="X20" s="40">
+        <v>4</v>
+      </c>
+      <c r="Y20" s="40">
+        <v>14000</v>
       </c>
     </row>
     <row r="21" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="S21" s="42"/>
-      <c r="W21" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="X21" s="41">
-        <v>3</v>
-      </c>
-      <c r="Y21" s="41">
-        <v>4500</v>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="S21" s="41"/>
+      <c r="W21" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="X21" s="40">
+        <v>6</v>
+      </c>
+      <c r="Y21" s="40">
+        <v>9000</v>
       </c>
     </row>
     <row r="22" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="30"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="26">
+        <v>1</v>
+      </c>
+      <c r="G22" s="42"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="29"/>
       <c r="Q22" s="3" t="str">
         <f>B22</f>
         <v>ca</v>
       </c>
       <c r="R22" s="3">
         <f>SUM(D22,F22,H22,J22,L22,N22,P22)</f>
-        <v>0</v>
-      </c>
-      <c r="S22" s="42">
+        <v>1</v>
+      </c>
+      <c r="S22" s="41">
         <f>LOOKUP(Q22,$W$7:$X$12)*R22</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="T22" s="3">
         <f>LOOKUP(Q22,$W$7:$X$12)</f>
@@ -2064,46 +2105,46 @@
         <f>INDEX($X$7:$X$12,MATCH(Q22,$W$7:$W$12,0))</f>
         <v>2000</v>
       </c>
-      <c r="W22" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="X22" s="41">
+      <c r="W22" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="X22" s="40">
         <v>1</v>
       </c>
-      <c r="Y22" s="41">
+      <c r="Y22" s="40">
         <v>1000</v>
       </c>
     </row>
     <row r="23" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="28">
+        <v>30</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="27">
         <v>2</v>
       </c>
-      <c r="I23" s="45"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="31"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="30"/>
       <c r="Q23" s="3" t="str">
-        <f t="shared" ref="Q23:Q24" si="9">B23</f>
+        <f t="shared" ref="Q23:Q24" si="10">B23</f>
         <v>cb</v>
       </c>
       <c r="R23" s="3">
         <f>SUM(D23,F23,H23,J23,L23,N23,P23)</f>
         <v>2</v>
       </c>
-      <c r="S23" s="42">
-        <f t="shared" ref="S23:S24" si="10">LOOKUP(Q23,$W$7:$X$12)*R23</f>
+      <c r="S23" s="41">
+        <f t="shared" ref="S23:S24" si="11">LOOKUP(Q23,$W$7:$X$12)*R23</f>
         <v>5000</v>
       </c>
       <c r="T23" s="3">
@@ -2111,45 +2152,45 @@
         <v>2500</v>
       </c>
       <c r="U23" s="3">
-        <f t="shared" ref="U23:U24" si="11">INDEX($X$7:$X$12,MATCH(Q23,$W$7:$W$12,0))</f>
+        <f t="shared" ref="U23:U24" si="12">INDEX($X$7:$X$12,MATCH(Q23,$W$7:$W$12,0))</f>
         <v>2500</v>
       </c>
-      <c r="W23" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="X23" s="41"/>
-      <c r="Y23" s="41"/>
+      <c r="W23" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="40"/>
     </row>
     <row r="24" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="29">
+        <v>24</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="28">
         <v>3</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="48"/>
-      <c r="P24" s="32"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="31"/>
       <c r="Q24" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>ce</v>
       </c>
       <c r="R24" s="3">
         <f>SUM(D24,F24,H24,J24,L24,N24,P24)</f>
         <v>3</v>
       </c>
-      <c r="S24" s="42">
-        <f t="shared" si="10"/>
+      <c r="S24" s="41">
+        <f t="shared" si="11"/>
         <v>4500</v>
       </c>
       <c r="T24" s="3">
@@ -2157,20 +2198,112 @@
         <v>1500</v>
       </c>
       <c r="U24" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1500</v>
       </c>
-      <c r="W24" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="X24" s="41">
-        <v>24</v>
-      </c>
-      <c r="Y24" s="41">
-        <v>56000</v>
-      </c>
+      <c r="W24" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="X24" s="40">
+        <v>34</v>
+      </c>
+      <c r="Y24" s="40">
+        <v>79000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="15"/>
+      <c r="C25" s="19" t="str">
+        <f ca="1">(TEXT(WeekStart+0+28,"mmm dd"))</f>
+        <v>May 29</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19" t="str">
+        <f ca="1">(TEXT(WeekStart+1+28,"mmm dd"))</f>
+        <v>May 30</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19" t="str">
+        <f ca="1">(TEXT(WeekStart+2+28,"mmm dd"))</f>
+        <v>May 31</v>
+      </c>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19" t="str">
+        <f ca="1">(TEXT(WeekStart+3+28,"mmm dd"))</f>
+        <v>Jun 01</v>
+      </c>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19" t="str">
+        <f ca="1">(TEXT(WeekStart+4+28,"mmm dd"))</f>
+        <v>Jun 02</v>
+      </c>
+      <c r="L25" s="19"/>
+      <c r="M25" s="21" t="str">
+        <f ca="1">(TEXT(WeekStart+5+28,"mmm dd"))</f>
+        <v>Jun 03</v>
+      </c>
+      <c r="N25" s="20"/>
+      <c r="O25" s="22" t="str">
+        <f ca="1">(TEXT(WeekStart+6+28,"mmm dd"))</f>
+        <v>Jun 04</v>
+      </c>
+      <c r="P25" s="20"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+    </row>
+    <row r="26" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
     </row>
     <row r="27" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="42"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="26">
+        <v>1</v>
+      </c>
+      <c r="I27" s="42"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="3" t="str">
+        <f>B27</f>
+        <v>ca</v>
+      </c>
+      <c r="R27" s="3">
+        <f>SUM(D27,F27,H27,J27,L27,N27,P27)</f>
+        <v>1</v>
+      </c>
+      <c r="S27" s="41">
+        <f>LOOKUP(Q27,$W$7:$X$12)*R27</f>
+        <v>2000</v>
+      </c>
       <c r="T27"/>
       <c r="U27"/>
       <c r="V27"/>
@@ -2189,6 +2322,37 @@
       <c r="AI27"/>
     </row>
     <row r="28" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="27">
+        <v>2</v>
+      </c>
+      <c r="I28" s="42"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="3" t="str">
+        <f t="shared" ref="Q28:Q29" si="13">B28</f>
+        <v>cb</v>
+      </c>
+      <c r="R28" s="3">
+        <f>SUM(D28,F28,H28,J28,L28,N28,P28)</f>
+        <v>2</v>
+      </c>
+      <c r="S28" s="41">
+        <f t="shared" ref="S28:S29" si="14">LOOKUP(Q28,$W$7:$X$12)*R28</f>
+        <v>5000</v>
+      </c>
       <c r="T28"/>
       <c r="U28"/>
       <c r="V28"/>
@@ -2207,6 +2371,37 @@
       <c r="AI28"/>
     </row>
     <row r="29" spans="2:35" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="42"/>
+      <c r="D29" s="28">
+        <v>3</v>
+      </c>
+      <c r="E29" s="42"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="3" t="str">
+        <f t="shared" si="13"/>
+        <v>ce</v>
+      </c>
+      <c r="R29" s="3">
+        <f>SUM(D29,F29,H29,J29,L29,N29,P29)</f>
+        <v>3</v>
+      </c>
+      <c r="S29" s="41">
+        <f t="shared" si="14"/>
+        <v>4500</v>
+      </c>
       <c r="T29"/>
       <c r="U29"/>
       <c r="V29"/>
@@ -2539,10 +2734,17 @@
       <c r="Q59"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="52">
     <mergeCell ref="Q5:Q6"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="S5:S6"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="E1:F1"/>
@@ -2550,6 +2752,7 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:H20"/>
@@ -2586,16 +2789,13 @@
     <mergeCell ref="I4:J4"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <dataValidations count="9">
+  <dataValidations xWindow="820" yWindow="305" count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Present" sqref="Q3:R4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Absent - excused" sqref="T3:U5 S3:S4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Student Name in this cell." sqref="I2:J2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Week Date in next cell G5." sqref="C1:D1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Week Date (i-e Monday Date) in this cell. Dates for Grid below will be auto-calculated." sqref="O3:P3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Homework Log" prompt="Help your students get more organized with this ready-to-print homework log to track their assignments. _x000a__x000a_" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the date for the start of the week in this cell." sqref="K2:L2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Homework Date header, these dates are calculated on basis of your input in cell D4." sqref="O15 O5 O10 C5 E5 G5 I5 K5 M5 C10 E10 G10 I10 K10 M10 C15 E15 G15 I15 K15 M15 C20 E20 G20 I20 K20 M20 O20"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Week Date (i.e., Monday Date) in this cell. Dates in Grid below will be auto-calculated." sqref="I1 K1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Homework Date header, these dates are calculated on basis of your input in cell D4." sqref="O15 O5 O10 C5 E5 G5 I5 K5 M5 C10 E10 G10 I10 K10 M10 C15 E15 G15 I15 K15 M15 C20 E20 G20 I20 K20 M20 O20 C25 E25 G25 I25 K25 M25 O25"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>